<commit_message>
added python file, added a reference to References.xlsx
</commit_message>
<xml_diff>
--- a/References.xlsx
+++ b/References.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammurphy/Computer Science/Third year/CSC3094 Dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC1855A-36C3-9840-82C2-86E98359CC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD5DAC0-5AFF-DD49-B276-B5206228087A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{6917758D-BE74-2741-A403-084D6158FD54}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="33600" windowHeight="20500" xr2:uid="{6917758D-BE74-2741-A403-084D6158FD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Author</t>
   </si>
@@ -54,13 +54,28 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Charles H. Bennett, Gilles Brassard,</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Quantum cryptography: Public key distribution and coin tossing, Theoretical Computer Science,</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.tcs.2014.05.025</t>
+  </si>
+  <si>
+    <t>Quantum cryptography, QKD, BB84 Protocol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,6 +85,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,16 +123,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -115,18 +182,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9F15525-5EC6-DC4A-AE96-FB39EB971EC7}" name="Table1" displayName="Table1" ref="A1:F16" totalsRowShown="0">
-  <autoFilter ref="A1:F16" xr:uid="{D9F15525-5EC6-DC4A-AE96-FB39EB971EC7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9F15525-5EC6-DC4A-AE96-FB39EB971EC7}" name="Table1" displayName="Table1" ref="A1:G16" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:G16" xr:uid="{D9F15525-5EC6-DC4A-AE96-FB39EB971EC7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F5">
     <sortCondition ref="A1:A16"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="13" xr3:uid="{EC3FAEAE-074D-754C-820D-F29F34B3038A}" name="ID"/>
-    <tableColumn id="1" xr3:uid="{4672AA95-B7F8-3A46-ADE5-FDBEC4182916}" name="Author"/>
-    <tableColumn id="2" xr3:uid="{BD876A57-B8B3-0740-8AB6-804CFC484F53}" name="Title"/>
-    <tableColumn id="3" xr3:uid="{71C822FA-4513-734D-945F-45E52330C77F}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{AD018B81-191F-BB40-A0DE-029CB28CF725}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{7A576501-E0F4-3B4E-A7B9-9792A16C8472}" name="Topic"/>
+  <tableColumns count="7">
+    <tableColumn id="13" xr3:uid="{EC3FAEAE-074D-754C-820D-F29F34B3038A}" name="ID" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{4672AA95-B7F8-3A46-ADE5-FDBEC4182916}" name="Author" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{BD876A57-B8B3-0740-8AB6-804CFC484F53}" name="Title" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{71C822FA-4513-734D-945F-45E52330C77F}" name="Year" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{AD018B81-191F-BB40-A0DE-029CB28CF725}" name="Description" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7A576501-E0F4-3B4E-A7B9-9792A16C8472}" name="Topic" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{F25492AF-ECA6-7E4A-B308-E2E4EF83C5BD}" name="Link" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -449,23 +517,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE0A9AE-2176-194D-BD29-7765FC231548}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="48.33203125" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -484,27 +553,171 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{9B63B17D-BDE9-D24F-B15E-6545F7C9682A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>